<commit_message>
adicionado os arquivos dml e dql 1.1
</commit_message>
<xml_diff>
--- a/1.0-exercicio-filmes/1.0-exercicio-filmes.xlsx
+++ b/1.0-exercicio-filmes/1.0-exercicio-filmes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\OneDrive\Desktop\exercicios-bd-sprint1\exercicios-sprint-1-bd\1.0-exercicio-filmes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FIC\Desktop\Bruno-atividades-bd-sprint-1\exercicios-sprint-1-bd\1.0-exercicio-filmes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{965793C4-3890-4D45-84CC-5278D277C479}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7F9F44-8A80-420F-A8C4-893FE7FF7289}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3948B117-A6C5-4789-847A-8E3F560AA066}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>